<commit_message>
paper ready for jiming
</commit_message>
<xml_diff>
--- a/abundance/MASTER_novocent_acefilter.xlsx
+++ b/abundance/MASTER_novocent_acefilter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33520" yWindow="6360" windowWidth="22440" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="-33600" yWindow="5000" windowWidth="22440" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>